<commit_message>
added hyphen support, working cover page
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aadikuchlous/Desktop/programming/Sikshana-text_to_vid/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9175BEA8-0415-D241-875F-882D7EF4EA38}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19E43E8E-FC87-3546-896A-91E1C0F49517}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -51,13 +51,13 @@
     <t>CAB* BAD* DAB*</t>
   </si>
   <si>
-    <t>C* A* B:* CAB</t>
-  </si>
-  <si>
-    <t>D* A* B:* DAB</t>
-  </si>
-  <si>
-    <t>B* A* D:* BAD</t>
+    <t>C* - A* - B:* CAB</t>
+  </si>
+  <si>
+    <t>B* - A* - D:* BAD</t>
+  </si>
+  <si>
+    <t>D* - A* - B:* DAB</t>
   </si>
 </sst>
 </file>
@@ -329,8 +329,8 @@
   </sheetPr>
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" zoomScale="209" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -365,18 +365,18 @@
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>